<commit_message>
Implementation of interface conductivities
</commit_message>
<xml_diff>
--- a/inputs/HeatSolverAnalyticalSolutions.xlsx
+++ b/inputs/HeatSolverAnalyticalSolutions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\C++\ALMOST\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D75D02-900A-4F0B-9F23-161AEDC7980F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BC946B-19B6-4B1A-A3C0-DBD5DE964F97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{B89BA52E-DB4C-4F8F-BAE4-806C00FF5CE4}"/>
   </bookViews>
@@ -4505,7 +4505,7 @@
   <dimension ref="C2:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4587,11 +4587,11 @@
         <v>30.588782813991656</v>
       </c>
       <c r="M4" s="4">
-        <v>30.856069999999999</v>
+        <v>30.856059999999999</v>
       </c>
       <c r="N4" s="4">
         <f>100*(L4-M4)/L4</f>
-        <v>-0.87380785183149678</v>
+        <v>-0.87377516010897738</v>
       </c>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.3">
@@ -4624,11 +4624,11 @@
         <v>50.211458153435842</v>
       </c>
       <c r="M5" s="4">
-        <v>49.436709999999998</v>
+        <v>49.436660000000003</v>
       </c>
       <c r="N5" s="4">
         <f t="shared" ref="N5:N23" si="4">100*(L5-M5)/L5</f>
-        <v>1.542970831614517</v>
+        <v>1.543070410479249</v>
       </c>
     </row>
     <row r="6" spans="3:14" x14ac:dyDescent="0.3">
@@ -4661,11 +4661,11 @@
         <v>67.33821280765153</v>
       </c>
       <c r="M6" s="4">
-        <v>65.856629999999996</v>
+        <v>65.856539999999995</v>
       </c>
       <c r="N6" s="4">
         <f t="shared" si="4"/>
-        <v>2.2002110627491804</v>
+        <v>2.200344716429977</v>
       </c>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.3">
@@ -4698,11 +4698,11 @@
         <v>82.092509521268425</v>
       </c>
       <c r="M7" s="4">
-        <v>80.150530000000003</v>
+        <v>80.150400000000005</v>
       </c>
       <c r="N7" s="4">
         <f t="shared" si="4"/>
-        <v>2.3655989232066252</v>
+        <v>2.3657572811381304</v>
       </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.3">
@@ -4735,11 +4735,11 @@
         <v>94.574245783979563</v>
       </c>
       <c r="M8" s="4">
-        <v>92.347719999999995</v>
+        <v>92.347549999999998</v>
       </c>
       <c r="N8" s="4">
         <f t="shared" si="4"/>
-        <v>2.354262268255626</v>
+        <v>2.3544420212090733</v>
       </c>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.3">
@@ -4773,11 +4773,11 @@
         <v>104.86358822963905</v>
       </c>
       <c r="M9" s="4">
-        <v>102.4726</v>
+        <v>102.47239999999999</v>
       </c>
       <c r="N9" s="4">
         <f t="shared" si="4"/>
-        <v>2.2800938533622017</v>
+        <v>2.2802845773335849</v>
       </c>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.3">
@@ -4810,11 +4810,11 @@
         <v>113.02380427492369</v>
       </c>
       <c r="M10" s="4">
-        <v>110.5449</v>
+        <v>110.54470000000001</v>
       </c>
       <c r="N10" s="4">
         <f t="shared" si="4"/>
-        <v>2.1932585713483022</v>
+        <v>2.1934355252221125</v>
       </c>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.3">
@@ -4841,11 +4841,11 @@
         <v>119.10334602545174</v>
       </c>
       <c r="M11" s="4">
-        <v>116.5802</v>
+        <v>116.58</v>
       </c>
       <c r="N11" s="4">
         <f t="shared" si="4"/>
-        <v>2.1184510004551464</v>
+        <v>2.1186189218500364</v>
       </c>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.3">
@@ -4854,7 +4854,7 @@
       </c>
       <c r="D12" s="4">
         <f>MAX(N4:N23)</f>
-        <v>2.7266793698010878</v>
+        <v>2.7268620904912941</v>
       </c>
       <c r="F12">
         <v>9</v>
@@ -4879,11 +4879,11 @@
         <v>123.13735789369559</v>
       </c>
       <c r="M12" s="4">
-        <v>120.59</v>
+        <v>120.5898</v>
       </c>
       <c r="N12" s="4">
         <f t="shared" si="4"/>
-        <v>2.0687124827663776</v>
+        <v>2.0688749030127007</v>
       </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.3">
@@ -4910,11 +4910,11 @@
         <v>125.14872291630638</v>
       </c>
       <c r="M13" s="4">
-        <v>122.5818</v>
+        <v>122.58150000000001</v>
       </c>
       <c r="N13" s="4">
         <f t="shared" si="4"/>
-        <v>2.0510979708702419</v>
+        <v>2.0513376856615757</v>
       </c>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.3">
@@ -4941,11 +4941,11 @@
         <v>125.14872291630638</v>
       </c>
       <c r="M14" s="4">
-        <v>122.55929999999999</v>
+        <v>122.559</v>
       </c>
       <c r="N14" s="4">
         <f t="shared" si="4"/>
-        <v>2.0690765802205386</v>
+        <v>2.0693162950118724</v>
       </c>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.3">
@@ -4972,11 +4972,11 @@
         <v>123.13735789369559</v>
       </c>
       <c r="M15" s="4">
-        <v>120.52249999999999</v>
+        <v>120.5222</v>
       </c>
       <c r="N15" s="4">
         <f t="shared" si="4"/>
-        <v>2.1235293158985962</v>
+        <v>2.123772946268069</v>
       </c>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.3">
@@ -5007,11 +5007,11 @@
         <v>119.10334602545174</v>
       </c>
       <c r="M16" s="4">
-        <v>116.4675</v>
+        <v>116.46729999999999</v>
       </c>
       <c r="N16" s="4">
         <f t="shared" si="4"/>
-        <v>2.2130747064725411</v>
+        <v>2.2132426278674311</v>
       </c>
     </row>
     <row r="17" spans="6:14" x14ac:dyDescent="0.3">
@@ -5038,11 +5038,11 @@
         <v>113.02380427492392</v>
       </c>
       <c r="M17" s="4">
-        <v>110.38679999999999</v>
+        <v>110.3866</v>
       </c>
       <c r="N17" s="4">
         <f t="shared" si="4"/>
-        <v>2.3331406086009663</v>
+        <v>2.3333175624747766</v>
       </c>
     </row>
     <row r="18" spans="6:14" x14ac:dyDescent="0.3">
@@ -5069,11 +5069,11 @@
         <v>104.86358822963905</v>
       </c>
       <c r="M18" s="4">
-        <v>102.2688</v>
+        <v>102.26860000000001</v>
       </c>
       <c r="N18" s="4">
         <f t="shared" si="4"/>
-        <v>2.4744415801953736</v>
+        <v>2.4746323041667435</v>
       </c>
     </row>
     <row r="19" spans="6:14" x14ac:dyDescent="0.3">
@@ -5100,11 +5100,11 @@
         <v>94.574245783979336</v>
       </c>
       <c r="M19" s="4">
-        <v>92.09787</v>
+        <v>92.09769</v>
       </c>
       <c r="N19" s="4">
         <f t="shared" si="4"/>
-        <v>2.6184462413115308</v>
+        <v>2.6186365679681254</v>
       </c>
     </row>
     <row r="20" spans="6:14" x14ac:dyDescent="0.3">
@@ -5131,11 +5131,11 @@
         <v>82.092509521268425</v>
       </c>
       <c r="M20" s="4">
-        <v>79.854110000000006</v>
+        <v>79.853960000000001</v>
       </c>
       <c r="N20" s="4">
         <f t="shared" si="4"/>
-        <v>2.7266793698010878</v>
+        <v>2.7268620904912941</v>
       </c>
     </row>
     <row r="21" spans="6:14" x14ac:dyDescent="0.3">
@@ -5162,11 +5162,11 @@
         <v>67.33821280765153</v>
       </c>
       <c r="M21" s="4">
-        <v>65.513040000000004</v>
+        <v>65.512929999999997</v>
       </c>
       <c r="N21" s="4">
         <f t="shared" si="4"/>
-        <v>2.7104562648032364</v>
+        <v>2.7106196193019976</v>
       </c>
     </row>
     <row r="22" spans="6:14" x14ac:dyDescent="0.3">
@@ -5193,11 +5193,11 @@
         <v>50.211458153435728</v>
       </c>
       <c r="M22" s="4">
-        <v>49.045229999999997</v>
+        <v>49.045160000000003</v>
       </c>
       <c r="N22" s="4">
         <f t="shared" si="4"/>
-        <v>2.3226335110045646</v>
+        <v>2.3227729214151922</v>
       </c>
     </row>
     <row r="23" spans="6:14" x14ac:dyDescent="0.3">
@@ -5224,11 +5224,11 @@
         <v>30.588782813991656</v>
       </c>
       <c r="M23" s="4">
-        <v>30.415859999999999</v>
+        <v>30.415839999999999</v>
       </c>
       <c r="N23" s="4">
         <f t="shared" si="4"/>
-        <v>0.56531446525084028</v>
+        <v>0.56537984869587921</v>
       </c>
     </row>
     <row r="24" spans="6:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
lots of bug fixes for the heat solvers
</commit_message>
<xml_diff>
--- a/inputs/HeatSolverAnalyticalSolutions.xlsx
+++ b/inputs/HeatSolverAnalyticalSolutions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\C++\ALMOST\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BC946B-19B6-4B1A-A3C0-DBD5DE964F97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902BCA80-8345-4145-83D2-0088051701E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{B89BA52E-DB4C-4F8F-BAE4-806C00FF5CE4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{B89BA52E-DB4C-4F8F-BAE4-806C00FF5CE4}"/>
   </bookViews>
   <sheets>
     <sheet name="heat1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="heat6" sheetId="8" r:id="rId6"/>
     <sheet name="heat7" sheetId="10" r:id="rId7"/>
     <sheet name="heat8" sheetId="12" r:id="rId8"/>
+    <sheet name="heat10" sheetId="14" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="26">
   <si>
     <t>cells</t>
   </si>
@@ -4504,8 +4505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D86483D6-782B-46AD-A96F-9F92954B158D}">
   <dimension ref="C2:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4587,11 +4588,11 @@
         <v>30.588782813991656</v>
       </c>
       <c r="M4" s="4">
-        <v>30.856059999999999</v>
+        <v>30.658840000000001</v>
       </c>
       <c r="N4" s="4">
         <f>100*(L4-M4)/L4</f>
-        <v>-0.87377516010897738</v>
+        <v>-0.2290290085563654</v>
       </c>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.3">
@@ -4624,11 +4625,11 @@
         <v>50.211458153435842</v>
       </c>
       <c r="M5" s="4">
-        <v>49.436660000000003</v>
+        <v>49.313220000000001</v>
       </c>
       <c r="N5" s="4">
         <f t="shared" ref="N5:N23" si="4">100*(L5-M5)/L5</f>
-        <v>1.543070410479249</v>
+        <v>1.7889107117562904</v>
       </c>
     </row>
     <row r="6" spans="3:14" x14ac:dyDescent="0.3">
@@ -4661,11 +4662,11 @@
         <v>67.33821280765153</v>
       </c>
       <c r="M6" s="4">
-        <v>65.856539999999995</v>
+        <v>65.786209999999997</v>
       </c>
       <c r="N6" s="4">
         <f t="shared" si="4"/>
-        <v>2.200344716429977</v>
+        <v>2.3047876427679435</v>
       </c>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.3">
@@ -4698,11 +4699,11 @@
         <v>82.092509521268425</v>
       </c>
       <c r="M7" s="4">
-        <v>80.150400000000005</v>
+        <v>80.115629999999996</v>
       </c>
       <c r="N7" s="4">
         <f t="shared" si="4"/>
-        <v>2.3657572811381304</v>
+        <v>2.4081119371265682</v>
       </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.3">
@@ -4735,11 +4736,11 @@
         <v>94.574245783979563</v>
       </c>
       <c r="M8" s="4">
-        <v>92.347549999999998</v>
+        <v>92.333569999999995</v>
       </c>
       <c r="N8" s="4">
         <f t="shared" si="4"/>
-        <v>2.3544420212090733</v>
+        <v>2.369224058204574</v>
       </c>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.3">
@@ -4773,11 +4774,11 @@
         <v>104.86358822963905</v>
       </c>
       <c r="M9" s="4">
-        <v>102.47239999999999</v>
+        <v>102.4669</v>
       </c>
       <c r="N9" s="4">
         <f t="shared" si="4"/>
-        <v>2.2802845773335849</v>
+        <v>2.2855294865464506</v>
       </c>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.3">
@@ -4810,11 +4811,11 @@
         <v>113.02380427492369</v>
       </c>
       <c r="M10" s="4">
-        <v>110.54470000000001</v>
+        <v>110.53789999999999</v>
       </c>
       <c r="N10" s="4">
         <f t="shared" si="4"/>
-        <v>2.1934355252221125</v>
+        <v>2.1994519569319073</v>
       </c>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.3">
@@ -4841,11 +4842,11 @@
         <v>119.10334602545174</v>
       </c>
       <c r="M11" s="4">
-        <v>116.58</v>
+        <v>116.56399999999999</v>
       </c>
       <c r="N11" s="4">
         <f t="shared" si="4"/>
-        <v>2.1186189218500364</v>
+        <v>2.1320526334407974</v>
       </c>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.3">
@@ -4854,7 +4855,7 @@
       </c>
       <c r="D12" s="4">
         <f>MAX(N4:N23)</f>
-        <v>2.7268620904912941</v>
+        <v>2.8850982082047523</v>
       </c>
       <c r="F12">
         <v>9</v>
@@ -4879,11 +4880,11 @@
         <v>123.13735789369559</v>
       </c>
       <c r="M12" s="4">
-        <v>120.5898</v>
+        <v>120.55889999999999</v>
       </c>
       <c r="N12" s="4">
         <f t="shared" si="4"/>
-        <v>2.0688749030127007</v>
+        <v>2.0939688310687816</v>
       </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.3">
@@ -4910,11 +4911,11 @@
         <v>125.14872291630638</v>
       </c>
       <c r="M13" s="4">
-        <v>122.58150000000001</v>
+        <v>122.532</v>
       </c>
       <c r="N13" s="4">
         <f t="shared" si="4"/>
-        <v>2.0513376856615757</v>
+        <v>2.0908906262322215</v>
       </c>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.3">
@@ -4941,11 +4942,11 @@
         <v>125.14872291630638</v>
       </c>
       <c r="M14" s="4">
-        <v>122.559</v>
+        <v>122.4888</v>
       </c>
       <c r="N14" s="4">
         <f t="shared" si="4"/>
-        <v>2.0693162950118724</v>
+        <v>2.1254095561847781</v>
       </c>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.3">
@@ -4972,11 +4973,11 @@
         <v>123.13735789369559</v>
       </c>
       <c r="M15" s="4">
-        <v>120.5222</v>
+        <v>120.43129999999999</v>
       </c>
       <c r="N15" s="4">
         <f t="shared" si="4"/>
-        <v>2.123772946268069</v>
+        <v>2.1975929482194498</v>
       </c>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.3">
@@ -5007,11 +5008,11 @@
         <v>119.10334602545174</v>
       </c>
       <c r="M16" s="4">
-        <v>116.46729999999999</v>
+        <v>116.3574</v>
       </c>
       <c r="N16" s="4">
         <f t="shared" si="4"/>
-        <v>2.2132426278674311</v>
+        <v>2.3055154343564368</v>
       </c>
     </row>
     <row r="17" spans="6:14" x14ac:dyDescent="0.3">
@@ -5038,11 +5039,11 @@
         <v>113.02380427492392</v>
       </c>
       <c r="M17" s="4">
-        <v>110.3866</v>
+        <v>110.26130000000001</v>
       </c>
       <c r="N17" s="4">
         <f t="shared" si="4"/>
-        <v>2.3333175624747766</v>
+        <v>2.4441791644212221</v>
       </c>
     </row>
     <row r="18" spans="6:14" x14ac:dyDescent="0.3">
@@ -5069,11 +5070,11 @@
         <v>104.86358822963905</v>
       </c>
       <c r="M18" s="4">
-        <v>102.26860000000001</v>
+        <v>102.1335</v>
       </c>
       <c r="N18" s="4">
         <f t="shared" si="4"/>
-        <v>2.4746323041667435</v>
+        <v>2.6034663468319201</v>
       </c>
     </row>
     <row r="19" spans="6:14" x14ac:dyDescent="0.3">
@@ -5100,11 +5101,11 @@
         <v>94.574245783979336</v>
       </c>
       <c r="M19" s="4">
-        <v>92.09769</v>
+        <v>91.960350000000005</v>
       </c>
       <c r="N19" s="4">
         <f t="shared" si="4"/>
-        <v>2.6186365679681254</v>
+        <v>2.7638558069496324</v>
       </c>
     </row>
     <row r="20" spans="6:14" x14ac:dyDescent="0.3">
@@ -5131,11 +5132,11 @@
         <v>82.092509521268425</v>
       </c>
       <c r="M20" s="4">
-        <v>79.853960000000001</v>
+        <v>79.724059999999994</v>
       </c>
       <c r="N20" s="4">
         <f t="shared" si="4"/>
-        <v>2.7268620904912941</v>
+        <v>2.8850982082047523</v>
       </c>
     </row>
     <row r="21" spans="6:14" x14ac:dyDescent="0.3">
@@ -5162,11 +5163,11 @@
         <v>67.33821280765153</v>
       </c>
       <c r="M21" s="4">
-        <v>65.512929999999997</v>
+        <v>65.402439999999999</v>
       </c>
       <c r="N21" s="4">
         <f t="shared" si="4"/>
-        <v>2.7106196193019976</v>
+        <v>2.8747017880931534</v>
       </c>
     </row>
     <row r="22" spans="6:14" x14ac:dyDescent="0.3">
@@ -5193,11 +5194,11 @@
         <v>50.211458153435728</v>
       </c>
       <c r="M22" s="4">
-        <v>49.045160000000003</v>
+        <v>48.96855</v>
       </c>
       <c r="N22" s="4">
         <f t="shared" si="4"/>
-        <v>2.3227729214151922</v>
+        <v>2.4753476579741229</v>
       </c>
     </row>
     <row r="23" spans="6:14" x14ac:dyDescent="0.3">
@@ -5224,11 +5225,11 @@
         <v>30.588782813991656</v>
       </c>
       <c r="M23" s="4">
-        <v>30.415839999999999</v>
+        <v>30.390319999999999</v>
       </c>
       <c r="N23" s="4">
         <f t="shared" si="4"/>
-        <v>0.56537984869587921</v>
+        <v>0.64880912456862516</v>
       </c>
     </row>
     <row r="24" spans="6:14" x14ac:dyDescent="0.3">
@@ -5332,4 +5333,702 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DBD4C4-7704-4BD1-9090-5D85E337D482}">
+  <dimension ref="C2:N37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" customWidth="1"/>
+    <col min="12" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="G2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <f>D8/2</f>
+        <v>0.01</v>
+      </c>
+      <c r="H4" s="4">
+        <f>$D$3+($D$4-$D$3)*LN($G4/$D$7)</f>
+        <v>128.2404601085629</v>
+      </c>
+      <c r="I4" s="4">
+        <v>31.129190000000001</v>
+      </c>
+      <c r="J4" s="4">
+        <f>100*(H4-I4)/H4</f>
+        <v>75.725921465310293</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5">
+        <v>22</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4">
+        <f>$G4+$D$8</f>
+        <v>0.03</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" ref="H5:H28" si="0">$D$3+($D$4-$D$3)*LN($G5/$D$7)</f>
+        <v>106.26821433520072</v>
+      </c>
+      <c r="I5" s="4">
+        <v>51.161729999999999</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" ref="J5:J23" si="1">100*(H5-I5)/H5</f>
+        <v>51.856036802668875</v>
+      </c>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>2000000</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6" s="4">
+        <f>$G5+$D$8</f>
+        <v>0.05</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" si="0"/>
+        <v>96.051701859880907</v>
+      </c>
+      <c r="I6" s="4">
+        <v>68.968440000000001</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="1"/>
+        <v>28.196545543138473</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7" s="4">
+        <f>$G6+$D$8</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="0"/>
+        <v>89.322257127456652</v>
+      </c>
+      <c r="I7" s="4">
+        <v>84.549300000000002</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="1"/>
+        <v>5.3435249857669538</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <f>D7/D9</f>
+        <v>0.02</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4">
+        <f>$G7+$D$8</f>
+        <v>9.0000000000000011E-2</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="0"/>
+        <v>84.295968561838535</v>
+      </c>
+      <c r="I8" s="4">
+        <v>97.904330000000002</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="1"/>
+        <v>-16.143549531883643</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>25</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9" s="4">
+        <f>$G8+$D$8</f>
+        <v>0.11000000000000001</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="0"/>
+        <v>80.282554652595508</v>
+      </c>
+      <c r="I9" s="4">
+        <v>109.0335</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" si="1"/>
+        <v>-35.81219540386784</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>7</v>
+      </c>
+      <c r="G10" s="4">
+        <f>$G9+$D$8</f>
+        <v>0.13</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="0"/>
+        <v>76.941472959332188</v>
+      </c>
+      <c r="I10" s="4">
+        <v>117.93689999999999</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" si="1"/>
+        <v>-53.281313008312374</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4">
+        <f>MAX(N4:N23)</f>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+      <c r="G11" s="4">
+        <f>$G10+$D$8</f>
+        <v>0.15</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" si="0"/>
+        <v>74.079456086518718</v>
+      </c>
+      <c r="I11" s="4">
+        <v>124.6144</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" si="1"/>
+        <v>-68.217217813344391</v>
+      </c>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <v>9</v>
+      </c>
+      <c r="G12" s="4">
+        <f>$G11+$D$8</f>
+        <v>0.16999999999999998</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" si="0"/>
+        <v>71.576193227438608</v>
+      </c>
+      <c r="I12" s="4">
+        <v>129.06610000000001</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="1"/>
+        <v>-80.319871985763484</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13" s="4">
+        <f>$G12+$D$8</f>
+        <v>0.18999999999999997</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" si="0"/>
+        <v>69.351680525234116</v>
+      </c>
+      <c r="I13" s="4">
+        <v>131.2919</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" si="1"/>
+        <v>-89.313220682847742</v>
+      </c>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>11</v>
+      </c>
+      <c r="G14" s="4">
+        <f>$G13+$D$8</f>
+        <v>0.20999999999999996</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" si="0"/>
+        <v>67.350011354094462</v>
+      </c>
+      <c r="I14" s="4">
+        <v>131.2919</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="1"/>
+        <v>-94.939685028008938</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>12</v>
+      </c>
+      <c r="G15" s="4">
+        <f>$G14+$D$8</f>
+        <v>0.22999999999999995</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" si="0"/>
+        <v>65.530575789979935</v>
+      </c>
+      <c r="I15" s="4">
+        <v>129.06610000000001</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="1"/>
+        <v>-96.955540896887825</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>13</v>
+      </c>
+      <c r="G16" s="4">
+        <f>$G15+$D$8</f>
+        <v>0.24999999999999994</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" si="0"/>
+        <v>63.862943611198908</v>
+      </c>
+      <c r="I16" s="4">
+        <v>124.6144</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" si="1"/>
+        <v>-95.127867513685686</v>
+      </c>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <v>14</v>
+      </c>
+      <c r="G17" s="4">
+        <f>$G16+$D$8</f>
+        <v>0.26999999999999996</v>
+      </c>
+      <c r="H17" s="4">
+        <f t="shared" si="0"/>
+        <v>62.323722788476346</v>
+      </c>
+      <c r="I17" s="4">
+        <v>117.93689999999999</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" si="1"/>
+        <v>-89.232758768714831</v>
+      </c>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+    </row>
+    <row r="18" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <v>15</v>
+      </c>
+      <c r="G18" s="4">
+        <f>$G17+$D$8</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H18" s="4">
+        <f t="shared" si="0"/>
+        <v>60.894543508833443</v>
+      </c>
+      <c r="I18" s="4">
+        <v>109.0335</v>
+      </c>
+      <c r="J18" s="4">
+        <f t="shared" si="1"/>
+        <v>-79.052988522992152</v>
+      </c>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <v>16</v>
+      </c>
+      <c r="G19" s="4">
+        <f>$G18+$D$8</f>
+        <v>0.31</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" si="0"/>
+        <v>59.560716018859992</v>
+      </c>
+      <c r="I19" s="4">
+        <v>97.904330000000002</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="1"/>
+        <v>-64.37735565334448</v>
+      </c>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>17</v>
+      </c>
+      <c r="G20" s="4">
+        <f>$G19+$D$8</f>
+        <v>0.33</v>
+      </c>
+      <c r="H20" s="4">
+        <f t="shared" si="0"/>
+        <v>58.310308879233318</v>
+      </c>
+      <c r="I20" s="4">
+        <v>84.549300000000002</v>
+      </c>
+      <c r="J20" s="4">
+        <f t="shared" si="1"/>
+        <v>-44.998888918785099</v>
+      </c>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <v>18</v>
+      </c>
+      <c r="G21" s="4">
+        <f>$G20+$D$8</f>
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="0"/>
+        <v>57.133498878774645</v>
+      </c>
+      <c r="I21" s="4">
+        <v>68.968440000000001</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="1"/>
+        <v>-20.714539374416102</v>
+      </c>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+    </row>
+    <row r="22" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>19</v>
+      </c>
+      <c r="G22" s="4">
+        <f>$G21+$D$8</f>
+        <v>0.37000000000000005</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" si="0"/>
+        <v>56.022101855678429</v>
+      </c>
+      <c r="I22" s="4">
+        <v>51.161729999999999</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="1"/>
+        <v>8.6758113221090802</v>
+      </c>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <v>20</v>
+      </c>
+      <c r="G23" s="4">
+        <f>$G22+$D$8</f>
+        <v>0.39000000000000007</v>
+      </c>
+      <c r="H23" s="4">
+        <f t="shared" si="0"/>
+        <v>54.969227185969991</v>
+      </c>
+      <c r="I23" s="4">
+        <v>31.129190000000001</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" si="1"/>
+        <v>43.369787800209018</v>
+      </c>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+    </row>
+    <row r="24" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <v>21</v>
+      </c>
+      <c r="G24" s="4">
+        <f t="shared" ref="G24:G28" si="2">$G23+$D$8</f>
+        <v>0.41000000000000009</v>
+      </c>
+      <c r="H24" s="4">
+        <f t="shared" si="0"/>
+        <v>53.969018774476758</v>
+      </c>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F25">
+        <v>22</v>
+      </c>
+      <c r="G25" s="4">
+        <f t="shared" si="2"/>
+        <v>0.4300000000000001</v>
+      </c>
+      <c r="H25" s="4">
+        <f t="shared" si="0"/>
+        <v>53.016457794691668</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F26">
+        <v>23</v>
+      </c>
+      <c r="G26" s="4">
+        <f t="shared" si="2"/>
+        <v>0.45000000000000012</v>
+      </c>
+      <c r="H26" s="4">
+        <f t="shared" si="0"/>
+        <v>52.107210313156521</v>
+      </c>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F27">
+        <v>24</v>
+      </c>
+      <c r="G27" s="4">
+        <f t="shared" si="2"/>
+        <v>0.47000000000000014</v>
+      </c>
+      <c r="H27" s="4">
+        <f t="shared" si="0"/>
+        <v>51.237508074361742</v>
+      </c>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F28">
+        <v>25</v>
+      </c>
+      <c r="G28" s="4">
+        <f t="shared" si="2"/>
+        <v>0.49000000000000016</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" si="0"/>
+        <v>50.404054146350383</v>
+      </c>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="H29" s="2"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Spherical heat solver implementation
</commit_message>
<xml_diff>
--- a/inputs/HeatSolverAnalyticalSolutions.xlsx
+++ b/inputs/HeatSolverAnalyticalSolutions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\C++\ALMOST\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B2963A-5DF6-44EB-AEC8-5B6FFC92DB38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB33D18-3326-4AB9-8A62-D876B6613B4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="13" xr2:uid="{B89BA52E-DB4C-4F8F-BAE4-806C00FF5CE4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="15" xr2:uid="{B89BA52E-DB4C-4F8F-BAE4-806C00FF5CE4}"/>
   </bookViews>
   <sheets>
     <sheet name="heat1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,8 @@
     <sheet name="heat12" sheetId="17" r:id="rId12"/>
     <sheet name="heat13" sheetId="19" r:id="rId13"/>
     <sheet name="heat14" sheetId="20" r:id="rId14"/>
+    <sheet name="heat15" sheetId="21" r:id="rId15"/>
+    <sheet name="heat16" sheetId="22" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -68,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="29">
   <si>
     <t>cells</t>
   </si>
@@ -5297,7 +5299,7 @@
   <dimension ref="C2:N37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="C2" sqref="C2:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7270,7 +7272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CDEB057-5746-44CF-A13F-97E2A5DA4D44}">
   <dimension ref="C2:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
@@ -7917,6 +7919,1477 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9637C3FC-AA45-4027-ADB2-452FFD54938F}">
+  <dimension ref="C2:N37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" customWidth="1"/>
+    <col min="12" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="G2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="5">
+        <v>22.003450000000001</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <f>D8/2</f>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="H4" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G4^2)</f>
+        <v>76.773767295583212</v>
+      </c>
+      <c r="I4" s="4">
+        <v>76.809269999999998</v>
+      </c>
+      <c r="J4" s="4">
+        <f>100*(H4-I4)/H4</f>
+        <v>-4.6243275102155833E-2</v>
+      </c>
+      <c r="L4" s="4">
+        <f>SQRT(1/($D$5^2)+2*$H4/$D$5)-1/$D$5</f>
+        <v>73.918093638825781</v>
+      </c>
+      <c r="M4" s="4">
+        <v>74.154979999999995</v>
+      </c>
+      <c r="N4" s="4">
+        <f>100*(L4-M4)/L4</f>
+        <v>-0.32047141574250326</v>
+      </c>
+    </row>
+    <row r="5" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>1.0452906248792999E-3</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4">
+        <f>$G4+$D$8</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="H5" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G5^2)</f>
+        <v>76.489720930126879</v>
+      </c>
+      <c r="I5" s="4">
+        <v>76.525229999999993</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" ref="J5:J23" si="0">100*(H5-I5)/H5</f>
+        <v>-4.6423322560624931E-2</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" ref="L5:L23" si="1">SQRT(1/($D$5^2)+2*$H5/$D$5)-1/$D$5</f>
+        <v>73.65438649508917</v>
+      </c>
+      <c r="M5" s="4">
+        <v>73.891329999999996</v>
+      </c>
+      <c r="N5" s="4">
+        <f t="shared" ref="N5:N23" si="2">100*(L5-M5)/L5</f>
+        <v>-0.32169639336636674</v>
+      </c>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>500000</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6" s="4">
+        <f>$G5+$D$8</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="H6" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G6^2)</f>
+        <v>75.921628199214226</v>
+      </c>
+      <c r="I6" s="4">
+        <v>75.957130000000006</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="0"/>
+        <v>-4.6761116203443379E-2</v>
+      </c>
+      <c r="L6" s="4">
+        <f t="shared" si="1"/>
+        <v>73.126769620070149</v>
+      </c>
+      <c r="M6" s="4">
+        <v>73.363839999999996</v>
+      </c>
+      <c r="N6" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.32419096476098297</v>
+      </c>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7">
+        <v>0.1</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7" s="4">
+        <f>$G6+$D$8</f>
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="H7" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G7^2)</f>
+        <v>75.069489102845239</v>
+      </c>
+      <c r="I7" s="4">
+        <v>75.104990000000001</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="0"/>
+        <v>-4.729071368279282E-2</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" si="1"/>
+        <v>72.334837059511187</v>
+      </c>
+      <c r="M7" s="4">
+        <v>72.572090000000003</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.32799263831011771</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <f>D7/D9</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4">
+        <f>$G7+$D$8</f>
+        <v>2.2500000000000003E-2</v>
+      </c>
+      <c r="H8" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G8^2)</f>
+        <v>73.933303641019933</v>
+      </c>
+      <c r="I8" s="4">
+        <v>73.968810000000005</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="0"/>
+        <v>-4.802485109075038E-2</v>
+      </c>
+      <c r="L8" s="4">
+        <f t="shared" si="1"/>
+        <v>71.277977927105326</v>
+      </c>
+      <c r="M8" s="4">
+        <v>71.515469999999993</v>
+      </c>
+      <c r="N8" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.33319137242858721</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9" s="4">
+        <f>$G8+$D$8</f>
+        <v>2.7500000000000004E-2</v>
+      </c>
+      <c r="H9" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G9^2)</f>
+        <v>72.513071813738307</v>
+      </c>
+      <c r="I9" s="4">
+        <v>72.548580000000001</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" si="0"/>
+        <v>-4.8967979667035415E-2</v>
+      </c>
+      <c r="L9" s="4">
+        <f t="shared" si="1"/>
+        <v>69.955374038864306</v>
+      </c>
+      <c r="M9" s="4">
+        <v>70.193169999999995</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.33992522290507515</v>
+      </c>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>7</v>
+      </c>
+      <c r="G10" s="4">
+        <f>$G9+$D$8</f>
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="H10" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G10^2)</f>
+        <v>70.808793621000348</v>
+      </c>
+      <c r="I10" s="4">
+        <v>70.844300000000004</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" si="0"/>
+        <v>-5.0144024751646019E-2</v>
+      </c>
+      <c r="L10" s="4">
+        <f t="shared" si="1"/>
+        <v>68.36599672571981</v>
+      </c>
+      <c r="M10" s="4">
+        <v>68.604159999999993</v>
+      </c>
+      <c r="N10" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.3483651020779806</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4" cm="1">
+        <f t="array" ref="D11">MAX(ABS(N4:N23))</f>
+        <v>1.042526956445005</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+      <c r="G11" s="4">
+        <f>$G10+$D$8</f>
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="H11" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G11^2)</f>
+        <v>68.820469062806069</v>
+      </c>
+      <c r="I11" s="4">
+        <v>68.855969999999999</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" si="0"/>
+        <v>-5.1584852119406374E-2</v>
+      </c>
+      <c r="L11" s="4">
+        <f t="shared" si="1"/>
+        <v>66.508602795183265</v>
+      </c>
+      <c r="M11" s="4">
+        <v>66.747200000000007</v>
+      </c>
+      <c r="N11" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.35874637985030955</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <v>9</v>
+      </c>
+      <c r="G12" s="4">
+        <f>$G11+$D$8</f>
+        <v>4.2499999999999996E-2</v>
+      </c>
+      <c r="H12" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G12^2)</f>
+        <v>66.548098139155456</v>
+      </c>
+      <c r="I12" s="4">
+        <v>66.583600000000004</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="0"/>
+        <v>-5.3347671589819824E-2</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" si="1"/>
+        <v>64.381729604708426</v>
+      </c>
+      <c r="M12" s="4">
+        <v>64.620819999999995</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.37136373433820252</v>
+      </c>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13" s="4">
+        <f>$G12+$D$8</f>
+        <v>4.7499999999999994E-2</v>
+      </c>
+      <c r="H13" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G13^2)</f>
+        <v>63.991680850048525</v>
+      </c>
+      <c r="I13" s="4">
+        <v>64.027190000000004</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" si="0"/>
+        <v>-5.5490259795938753E-2</v>
+      </c>
+      <c r="L13" s="4">
+        <f t="shared" si="1"/>
+        <v>61.98368920057942</v>
+      </c>
+      <c r="M13" s="4">
+        <v>62.22334</v>
+      </c>
+      <c r="N13" s="4">
+        <f>100*(L13-M13)/L13</f>
+        <v>-0.38663526245601448</v>
+      </c>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>11</v>
+      </c>
+      <c r="G14" s="4">
+        <f>$G13+$D$8</f>
+        <v>5.2499999999999991E-2</v>
+      </c>
+      <c r="H14" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G14^2)</f>
+        <v>61.151217195485266</v>
+      </c>
+      <c r="I14" s="4">
+        <v>61.186720000000001</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="0"/>
+        <v>-5.8057396308631631E-2</v>
+      </c>
+      <c r="L14" s="4">
+        <f t="shared" si="1"/>
+        <v>59.312561466551074</v>
+      </c>
+      <c r="M14" s="4">
+        <v>59.552840000000003</v>
+      </c>
+      <c r="N14" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.40510564289898854</v>
+      </c>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>12</v>
+      </c>
+      <c r="G15" s="4">
+        <f>$G14+$D$8</f>
+        <v>5.7499999999999989E-2</v>
+      </c>
+      <c r="H15" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G15^2)</f>
+        <v>58.026707175465681</v>
+      </c>
+      <c r="I15" s="4">
+        <v>58.06221</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="0"/>
+        <v>-6.1183593318440387E-2</v>
+      </c>
+      <c r="L15" s="4">
+        <f t="shared" si="1"/>
+        <v>56.366186215887751</v>
+      </c>
+      <c r="M15" s="4">
+        <v>56.607149999999997</v>
+      </c>
+      <c r="N15" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.42749705149348277</v>
+      </c>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>13</v>
+      </c>
+      <c r="G16" s="4">
+        <f>$G15+$D$8</f>
+        <v>6.2499999999999986E-2</v>
+      </c>
+      <c r="H16" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G16^2)</f>
+        <v>54.61815078998977</v>
+      </c>
+      <c r="I16" s="4">
+        <v>54.653660000000002</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" si="0"/>
+        <v>-6.5013570574309079E-2</v>
+      </c>
+      <c r="L16" s="4">
+        <f t="shared" si="1"/>
+        <v>53.142154148691361</v>
+      </c>
+      <c r="M16" s="4">
+        <v>53.383879999999998</v>
+      </c>
+      <c r="N16" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.45486649004157698</v>
+      </c>
+    </row>
+    <row r="17" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <v>14</v>
+      </c>
+      <c r="G17" s="4">
+        <f>$G16+$D$8</f>
+        <v>6.7499999999999991E-2</v>
+      </c>
+      <c r="H17" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G17^2)</f>
+        <v>50.925548039057531</v>
+      </c>
+      <c r="I17" s="4">
+        <v>50.96105</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" si="0"/>
+        <v>-6.9713458783478108E-2</v>
+      </c>
+      <c r="L17" s="4">
+        <f t="shared" si="1"/>
+        <v>49.637796583225281</v>
+      </c>
+      <c r="M17" s="4">
+        <v>49.880360000000003</v>
+      </c>
+      <c r="N17" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.48866676901749184</v>
+      </c>
+    </row>
+    <row r="18" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <v>15</v>
+      </c>
+      <c r="G18" s="4">
+        <f>$G17+$D$8</f>
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="H18" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G18^2)</f>
+        <v>46.94889892266896</v>
+      </c>
+      <c r="I18" s="4">
+        <v>46.984400000000001</v>
+      </c>
+      <c r="J18" s="4">
+        <f t="shared" si="0"/>
+        <v>-7.561642156830152E-2</v>
+      </c>
+      <c r="L18" s="4">
+        <f t="shared" si="1"/>
+        <v>45.850173855046137</v>
+      </c>
+      <c r="M18" s="4">
+        <v>46.093640000000001</v>
+      </c>
+      <c r="N18" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.53100375523890975</v>
+      </c>
+    </row>
+    <row r="19" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <v>16</v>
+      </c>
+      <c r="G19" s="4">
+        <f>$G18+$D$8</f>
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="H19" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G19^2)</f>
+        <v>42.688203440824061</v>
+      </c>
+      <c r="I19" s="4">
+        <v>42.723709999999997</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="0"/>
+        <v>-8.3176513214373318E-2</v>
+      </c>
+      <c r="L19" s="4">
+        <f t="shared" si="1"/>
+        <v>41.776062260817071</v>
+      </c>
+      <c r="M19" s="4">
+        <v>42.020499999999998</v>
+      </c>
+      <c r="N19" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.58511435964655945</v>
+      </c>
+    </row>
+    <row r="20" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>17</v>
+      </c>
+      <c r="G20" s="4">
+        <f>$G19+$D$8</f>
+        <v>8.2500000000000004E-2</v>
+      </c>
+      <c r="H20" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G20^2)</f>
+        <v>38.143461593522844</v>
+      </c>
+      <c r="I20" s="4">
+        <v>38.17897</v>
+      </c>
+      <c r="J20" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.3091725275363385E-2</v>
+      </c>
+      <c r="L20" s="4">
+        <f t="shared" si="1"/>
+        <v>37.411939404280702</v>
+      </c>
+      <c r="M20" s="4">
+        <v>37.657429999999998</v>
+      </c>
+      <c r="N20" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.65618249047844635</v>
+      </c>
+    </row>
+    <row r="21" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <v>18</v>
+      </c>
+      <c r="G21" s="4">
+        <f>$G20+$D$8</f>
+        <v>8.7500000000000008E-2</v>
+      </c>
+      <c r="H21" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G21^2)</f>
+        <v>33.314673380765292</v>
+      </c>
+      <c r="I21" s="4">
+        <v>33.350180000000002</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.10657952076819641</v>
+      </c>
+      <c r="L21" s="4">
+        <f t="shared" si="1"/>
+        <v>32.753967779553022</v>
+      </c>
+      <c r="M21" s="4">
+        <v>33.000590000000003</v>
+      </c>
+      <c r="N21" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.75295372489477874</v>
+      </c>
+    </row>
+    <row r="22" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>19</v>
+      </c>
+      <c r="G22" s="4">
+        <f>$G21+$D$8</f>
+        <v>9.2500000000000013E-2</v>
+      </c>
+      <c r="H22" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G22^2)</f>
+        <v>28.201838802551411</v>
+      </c>
+      <c r="I22" s="4">
+        <v>28.23734</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.12588256282557456</v>
+      </c>
+      <c r="L22" s="4">
+        <f t="shared" si="1"/>
+        <v>27.797976401067444</v>
+      </c>
+      <c r="M22" s="4">
+        <v>28.045809999999999</v>
+      </c>
+      <c r="N22" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.89155266324723637</v>
+      </c>
+    </row>
+    <row r="23" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <v>20</v>
+      </c>
+      <c r="G23" s="4">
+        <f>$G22+$D$8</f>
+        <v>9.7500000000000017E-2</v>
+      </c>
+      <c r="H23" s="4">
+        <f>$D$3+($D$6/(4*$D$4))*($D$7^2-$G23^2)</f>
+        <v>22.804957858881217</v>
+      </c>
+      <c r="I23" s="4">
+        <v>22.84046</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.15567729323804663</v>
+      </c>
+      <c r="L23" s="4">
+        <f t="shared" si="1"/>
+        <v>22.539440259463277</v>
+      </c>
+      <c r="M23" s="4">
+        <v>22.774419999999999</v>
+      </c>
+      <c r="N23" s="4">
+        <f t="shared" si="2"/>
+        <v>-1.042526956445005</v>
+      </c>
+    </row>
+    <row r="24" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="H29" s="2"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50054ECD-1B3C-46D9-9663-7D0F170ED22B}">
+  <dimension ref="C2:N37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" customWidth="1"/>
+    <col min="12" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="G2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="5">
+        <v>22</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <f>D7/2</f>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="H4" s="4">
+        <f>$D$3+($D$5/(6*$D$4))*($D$6^2-$G4^2)</f>
+        <v>171.42045454545459</v>
+      </c>
+      <c r="I4" s="4">
+        <v>170.83850000000001</v>
+      </c>
+      <c r="J4" s="4">
+        <f>100*(H4-I4)/H4</f>
+        <v>0.3394895591647526</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>2000000</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" ref="G5:G23" si="0">$G4+$D$7</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" ref="H5:H23" si="1">$D$3+($D$5/(6*$D$4))*($D$6^2-$G5^2)</f>
+        <v>170.66287878787881</v>
+      </c>
+      <c r="I5" s="4">
+        <v>170.27029999999999</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" ref="J5:J23" si="2">100*(H5-I5)/H5</f>
+        <v>0.23003173898570209</v>
+      </c>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>0.1</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="0"/>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" si="1"/>
+        <v>169.14772727272731</v>
+      </c>
+      <c r="I6" s="4">
+        <v>168.84989999999999</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="2"/>
+        <v>0.17607524353378548</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <f>D6/D8</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="0"/>
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="1"/>
+        <v>166.87500000000006</v>
+      </c>
+      <c r="I7" s="4">
+        <v>166.6403</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="2"/>
+        <v>0.14064419475659054</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>2.2500000000000003E-2</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="1"/>
+        <v>163.844696969697</v>
+      </c>
+      <c r="I8" s="4">
+        <v>163.65729999999999</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="2"/>
+        <v>0.11437475436367893</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>2.7500000000000004E-2</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="1"/>
+        <v>160.05681818181822</v>
+      </c>
+      <c r="I9" s="4">
+        <v>159.90729999999999</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" si="2"/>
+        <v>9.3415690450860039E-2</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="4">
+        <f>MAX(J4:J23)</f>
+        <v>0.3394895591647526</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="0"/>
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="1"/>
+        <v>155.51136363636368</v>
+      </c>
+      <c r="I10" s="4">
+        <v>155.39340000000001</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" si="2"/>
+        <v>7.5855316039480175E-2</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <v>8</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="0"/>
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" si="1"/>
+        <v>150.20833333333337</v>
+      </c>
+      <c r="I11" s="4">
+        <v>150.1174</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" si="2"/>
+        <v>6.0538141470203186E-2</v>
+      </c>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <v>9</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>4.2499999999999996E-2</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" si="1"/>
+        <v>144.14772727272731</v>
+      </c>
+      <c r="I12" s="4">
+        <v>144.0805</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="2"/>
+        <v>4.6637761135223665E-2</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="0"/>
+        <v>4.7499999999999994E-2</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" si="1"/>
+        <v>137.3295454545455</v>
+      </c>
+      <c r="I13" s="4">
+        <v>137.2834</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" si="2"/>
+        <v>3.3601985933004626E-2</v>
+      </c>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>11</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="0"/>
+        <v>5.2499999999999991E-2</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" si="1"/>
+        <v>129.75378787878793</v>
+      </c>
+      <c r="I14" s="4">
+        <v>129.72659999999999</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="2"/>
+        <v>2.095343745443462E-2</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>12</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="0"/>
+        <v>5.7499999999999989E-2</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" si="1"/>
+        <v>121.4204545454546</v>
+      </c>
+      <c r="I15" s="4">
+        <v>121.4104</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="2"/>
+        <v>8.2807674310294583E-3</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>13</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="0"/>
+        <v>6.2499999999999986E-2</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" si="1"/>
+        <v>112.32954545454551</v>
+      </c>
+      <c r="I16" s="4">
+        <v>112.3353</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" si="2"/>
+        <v>-5.12291350526492E-3</v>
+      </c>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <v>14</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="0"/>
+        <v>6.7499999999999991E-2</v>
+      </c>
+      <c r="H17" s="4">
+        <f t="shared" si="1"/>
+        <v>102.48106060606065</v>
+      </c>
+      <c r="I17" s="4">
+        <v>102.5014</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" si="2"/>
+        <v>-1.984697837733861E-2</v>
+      </c>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+    </row>
+    <row r="18" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <v>15</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" si="0"/>
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="H18" s="4">
+        <f t="shared" si="1"/>
+        <v>91.875000000000043</v>
+      </c>
+      <c r="I18" s="4">
+        <v>91.908869999999993</v>
+      </c>
+      <c r="J18" s="4">
+        <f t="shared" si="2"/>
+        <v>-3.6865306122395143E-2</v>
+      </c>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <v>16</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="0"/>
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" si="1"/>
+        <v>80.511363636363654</v>
+      </c>
+      <c r="I19" s="4">
+        <v>80.557860000000005</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="2"/>
+        <v>-5.7751305575142679E-2</v>
+      </c>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>17</v>
+      </c>
+      <c r="G20" s="4">
+        <f t="shared" si="0"/>
+        <v>8.2500000000000004E-2</v>
+      </c>
+      <c r="H20" s="4">
+        <f t="shared" si="1"/>
+        <v>68.39015151515153</v>
+      </c>
+      <c r="I20" s="4">
+        <v>68.448480000000004</v>
+      </c>
+      <c r="J20" s="4">
+        <f t="shared" si="2"/>
+        <v>-8.5287842702836153E-2</v>
+      </c>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <v>18</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="0"/>
+        <v>8.7500000000000008E-2</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="1"/>
+        <v>55.51136363636364</v>
+      </c>
+      <c r="I21" s="4">
+        <v>55.580840000000002</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.12515701125895265</v>
+      </c>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+    </row>
+    <row r="22" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>19</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" si="0"/>
+        <v>9.2500000000000013E-2</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" si="1"/>
+        <v>41.874999999999986</v>
+      </c>
+      <c r="I22" s="4">
+        <v>41.954990000000002</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.19102089552242738</v>
+      </c>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <v>20</v>
+      </c>
+      <c r="G23" s="4">
+        <f t="shared" si="0"/>
+        <v>9.7500000000000017E-2</v>
+      </c>
+      <c r="H23" s="4">
+        <f t="shared" si="1"/>
+        <v>27.481060606060598</v>
+      </c>
+      <c r="I23" s="4">
+        <v>27.571020000000001</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.3273505168849376</v>
+      </c>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+    </row>
+    <row r="24" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="H29" s="2"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11549,7 +13022,7 @@
   <dimension ref="C2:N37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="C5" sqref="C5:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Last basic tests for the spherical heat solver
</commit_message>
<xml_diff>
--- a/inputs/HeatSolverAnalyticalSolutions.xlsx
+++ b/inputs/HeatSolverAnalyticalSolutions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\C++\ALMOST\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB33D18-3326-4AB9-8A62-D876B6613B4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C873A29E-E85C-4598-BA47-A678614B1FB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="15" xr2:uid="{B89BA52E-DB4C-4F8F-BAE4-806C00FF5CE4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="16" xr2:uid="{B89BA52E-DB4C-4F8F-BAE4-806C00FF5CE4}"/>
   </bookViews>
   <sheets>
     <sheet name="heat1" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="heat14" sheetId="20" r:id="rId14"/>
     <sheet name="heat15" sheetId="21" r:id="rId15"/>
     <sheet name="heat16" sheetId="22" r:id="rId16"/>
+    <sheet name="heat17" sheetId="23" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -70,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="29">
   <si>
     <t>cells</t>
   </si>
@@ -8750,7 +8751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50054ECD-1B3C-46D9-9663-7D0F170ED22B}">
   <dimension ref="C2:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
@@ -9285,6 +9286,659 @@
       <c r="J23" s="4">
         <f t="shared" si="2"/>
         <v>-0.3273505168849376</v>
+      </c>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+    </row>
+    <row r="24" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="H29" s="2"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA2EDF9-F4DD-4FA3-9A1A-CFFE76DCA797}">
+  <dimension ref="C2:N37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" customWidth="1"/>
+    <col min="12" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="G2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4">
+        <v>20000</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <f>D8/2</f>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="H4" s="4">
+        <f>$D$3+($D$5/(3*$D$4))*$D$7+($D$6/(6*$D$5))*($D$7^2-$G4^2)</f>
+        <v>171.42049121212125</v>
+      </c>
+      <c r="I4" s="4">
+        <v>171.17160000000001</v>
+      </c>
+      <c r="J4" s="4">
+        <f>100*(H4-I4)/H4</f>
+        <v>0.14519338403554716</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5">
+        <v>22</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4">
+        <f>$G4+$D$8</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" ref="H5:H23" si="0">$D$3+($D$5/(3*$D$4))*$D$7+($D$6/(6*$D$5))*($D$7^2-$G5^2)</f>
+        <v>170.66291545454547</v>
+      </c>
+      <c r="I5" s="4">
+        <v>170.60339999999999</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" ref="J5:J23" si="1">100*(H5-I5)/H5</f>
+        <v>3.4873103150126095E-2</v>
+      </c>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>2000000</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6" s="4">
+        <f>$G5+$D$8</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" si="0"/>
+        <v>169.14776393939397</v>
+      </c>
+      <c r="I6" s="4">
+        <v>169.18299999999999</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.0831526107935799E-2</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7">
+        <v>0.1</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7" s="4">
+        <f>$G6+$D$8</f>
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="0"/>
+        <v>166.87503666666672</v>
+      </c>
+      <c r="I7" s="4">
+        <v>166.9734</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="1"/>
+        <v>-5.894430664891049E-2</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <f>D7/D9</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4">
+        <f>$G7+$D$8</f>
+        <v>2.2500000000000003E-2</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="0"/>
+        <v>163.84473363636366</v>
+      </c>
+      <c r="I8" s="4">
+        <v>163.99039999999999</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="1"/>
+        <v>-8.8905124017979537E-2</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9" s="4">
+        <f>$G8+$D$8</f>
+        <v>2.7500000000000004E-2</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="0"/>
+        <v>160.05685484848487</v>
+      </c>
+      <c r="I9" s="4">
+        <v>160.24039999999999</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.11467497077139814</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>7</v>
+      </c>
+      <c r="G10" s="4">
+        <f>$G9+$D$8</f>
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="0"/>
+        <v>155.51140030303034</v>
+      </c>
+      <c r="I10" s="4">
+        <v>155.72649999999999</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.13831763880365081</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4">
+        <f>MAX(J4:J23)</f>
+        <v>0.14519338403554716</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+      <c r="G11" s="4">
+        <f>$G10+$D$8</f>
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" si="0"/>
+        <v>150.20837000000003</v>
+      </c>
+      <c r="I11" s="4">
+        <v>150.45060000000001</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.16126265134225071</v>
+      </c>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <v>9</v>
+      </c>
+      <c r="G12" s="4">
+        <f>$G11+$D$8</f>
+        <v>4.2499999999999996E-2</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" si="0"/>
+        <v>144.147763939394</v>
+      </c>
+      <c r="I12" s="4">
+        <v>144.4136</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.18441913585130243</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13" s="4">
+        <f>$G12+$D$8</f>
+        <v>4.7499999999999994E-2</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" si="0"/>
+        <v>137.32958212121216</v>
+      </c>
+      <c r="I13" s="4">
+        <v>137.6165</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.20892649227942928</v>
+      </c>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>11</v>
+      </c>
+      <c r="G14" s="4">
+        <f>$G13+$D$8</f>
+        <v>5.2499999999999991E-2</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" si="0"/>
+        <v>129.75382454545459</v>
+      </c>
+      <c r="I14" s="4">
+        <v>130.05969999999999</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.23573521290561134</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>12</v>
+      </c>
+      <c r="G15" s="4">
+        <f>$G14+$D$8</f>
+        <v>5.7499999999999989E-2</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" si="0"/>
+        <v>121.42049121212128</v>
+      </c>
+      <c r="I15" s="4">
+        <v>121.7436</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.26610729758476542</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>13</v>
+      </c>
+      <c r="G16" s="4">
+        <f>$G15+$D$8</f>
+        <v>6.2499999999999986E-2</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" si="0"/>
+        <v>112.32958212121218</v>
+      </c>
+      <c r="I16" s="4">
+        <v>112.66840000000001</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.3016283621728526</v>
+      </c>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <v>14</v>
+      </c>
+      <c r="G17" s="4">
+        <f>$G16+$D$8</f>
+        <v>6.7499999999999991E-2</v>
+      </c>
+      <c r="H17" s="4">
+        <f t="shared" si="0"/>
+        <v>102.48109727272731</v>
+      </c>
+      <c r="I17" s="4">
+        <v>102.83450000000001</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.34484674410950467</v>
+      </c>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+    </row>
+    <row r="18" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <v>15</v>
+      </c>
+      <c r="G18" s="4">
+        <f>$G17+$D$8</f>
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="H18" s="4">
+        <f t="shared" si="0"/>
+        <v>91.875036666666716</v>
+      </c>
+      <c r="I18" s="4">
+        <v>92.241990000000001</v>
+      </c>
+      <c r="J18" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.39940482926241899</v>
+      </c>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <v>16</v>
+      </c>
+      <c r="G19" s="4">
+        <f>$G18+$D$8</f>
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" si="0"/>
+        <v>80.511400303030328</v>
+      </c>
+      <c r="I19" s="4">
+        <v>80.890979999999999</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.47146080622247499</v>
+      </c>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>17</v>
+      </c>
+      <c r="G20" s="4">
+        <f>$G19+$D$8</f>
+        <v>8.2500000000000004E-2</v>
+      </c>
+      <c r="H20" s="4">
+        <f t="shared" si="0"/>
+        <v>68.390188181818203</v>
+      </c>
+      <c r="I20" s="4">
+        <v>68.781610000000001</v>
+      </c>
+      <c r="J20" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.57233622042563448</v>
+      </c>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <v>18</v>
+      </c>
+      <c r="G21" s="4">
+        <f>$G20+$D$8</f>
+        <v>8.7500000000000008E-2</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="0"/>
+        <v>55.511400303030307</v>
+      </c>
+      <c r="I21" s="4">
+        <v>55.913960000000003</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.72518382669536263</v>
+      </c>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+    </row>
+    <row r="22" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>19</v>
+      </c>
+      <c r="G22" s="4">
+        <f>$G21+$D$8</f>
+        <v>9.2500000000000013E-2</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" si="0"/>
+        <v>41.875036666666645</v>
+      </c>
+      <c r="I22" s="4">
+        <v>42.288119999999999</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.98646679791966985</v>
+      </c>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <v>20</v>
+      </c>
+      <c r="G23" s="4">
+        <f>$G22+$D$8</f>
+        <v>9.7500000000000017E-2</v>
+      </c>
+      <c r="H23" s="4">
+        <f t="shared" si="0"/>
+        <v>27.481097272727265</v>
+      </c>
+      <c r="I23" s="4">
+        <v>27.904150000000001</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.5394317158237405</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>

</xml_diff>